<commit_message>
Five More Measures of Bohemian Rhapsody
</commit_message>
<xml_diff>
--- a/HW4/Lines to Seconds stats.xlsx
+++ b/HW4/Lines to Seconds stats.xlsx
@@ -197,7 +197,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1112</c:v>
+                  <c:v>1592</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>897</c:v>
@@ -230,7 +230,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>123</c:v>
+                  <c:v>166</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>237</c:v>
@@ -296,7 +296,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1112</c:v>
+                  <c:v>1592</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>897</c:v>
@@ -329,28 +329,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>168.61398658135971</c:v>
+                  <c:v>205.81522640233038</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140.99187240585837</c:v>
+                  <c:v>131.95595884158342</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>67.632676153712936</c:v>
+                  <c:v>71.274459881602851</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.944439747269378</c:v>
+                  <c:v>42.580931476708358</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>145.7454455430377</c:v>
+                  <c:v>135.88803495632823</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>65.191652110296531</c:v>
+                  <c:v>69.255285660517686</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>51.18788259806562</c:v>
+                  <c:v>57.671601971134351</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>83.692044860399761</c:v>
+                  <c:v>84.558500809794751</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1394,7 +1394,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1415,34 +1415,34 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1112</v>
+        <v>1592</v>
       </c>
       <c r="C2">
-        <v>123</v>
+        <v>166</v>
       </c>
       <c r="D2">
         <f>B2*C2</f>
-        <v>136776</v>
+        <v>264272</v>
       </c>
       <c r="E2">
         <f>B2^2</f>
-        <v>1236544</v>
+        <v>2534464</v>
       </c>
       <c r="F2">
         <f>C2^2</f>
-        <v>15129</v>
+        <v>27556</v>
       </c>
       <c r="G2">
         <f t="shared" ref="G2:G7" si="0">G3</f>
-        <v>25.749842566673678</v>
+        <v>36.62968114087839</v>
       </c>
       <c r="H2">
         <f t="shared" ref="H2:H7" si="1">H3</f>
-        <v>0.12847494965349465</v>
+        <v>0.10627232742553516</v>
       </c>
       <c r="I2">
         <f>G2+H2*B2</f>
-        <v>168.61398658135971</v>
+        <v>205.81522640233038</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1469,15 +1469,15 @@
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
-        <v>25.749842566673678</v>
+        <v>36.62968114087839</v>
       </c>
       <c r="H3">
         <f t="shared" si="1"/>
-        <v>0.12847494965349465</v>
+        <v>0.10627232742553516</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I9" si="5">G3+H3*B3</f>
-        <v>140.99187240585837</v>
+        <v>131.95595884158342</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1504,15 +1504,15 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>25.749842566673678</v>
+        <v>36.62968114087839</v>
       </c>
       <c r="H4">
         <f t="shared" si="1"/>
-        <v>0.12847494965349465</v>
+        <v>0.10627232742553516</v>
       </c>
       <c r="I4">
         <f t="shared" si="5"/>
-        <v>67.632676153712936</v>
+        <v>71.274459881602851</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1539,15 +1539,15 @@
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>25.749842566673678</v>
+        <v>36.62968114087839</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
-        <v>0.12847494965349465</v>
+        <v>0.10627232742553516</v>
       </c>
       <c r="I5">
         <f t="shared" si="5"/>
-        <v>32.944439747269378</v>
+        <v>42.580931476708358</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1574,15 +1574,15 @@
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>25.749842566673678</v>
+        <v>36.62968114087839</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>0.12847494965349465</v>
+        <v>0.10627232742553516</v>
       </c>
       <c r="I6">
         <f t="shared" si="5"/>
-        <v>145.7454455430377</v>
+        <v>135.88803495632823</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1609,15 +1609,15 @@
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>25.749842566673678</v>
+        <v>36.62968114087839</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>0.12847494965349465</v>
+        <v>0.10627232742553516</v>
       </c>
       <c r="I7">
         <f t="shared" si="5"/>
-        <v>65.191652110296531</v>
+        <v>69.255285660517686</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1644,15 +1644,15 @@
       </c>
       <c r="G8">
         <f>G9</f>
-        <v>25.749842566673678</v>
+        <v>36.62968114087839</v>
       </c>
       <c r="H8">
         <f>H9</f>
-        <v>0.12847494965349465</v>
+        <v>0.10627232742553516</v>
       </c>
       <c r="I8">
         <f t="shared" si="5"/>
-        <v>51.18788259806562</v>
+        <v>57.671601971134351</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1679,15 +1679,15 @@
       </c>
       <c r="G9">
         <f>C10/8-H9*B10/8</f>
-        <v>25.749842566673678</v>
+        <v>36.62968114087839</v>
       </c>
       <c r="H9">
         <f>(8*D10-B10*C10)/(8*E10-B10^2)</f>
-        <v>0.12847494965349465</v>
+        <v>0.10627232742553516</v>
       </c>
       <c r="I9">
         <f t="shared" si="5"/>
-        <v>83.692044860399761</v>
+        <v>84.558500809794751</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1696,23 +1696,23 @@
       </c>
       <c r="B10">
         <f>SUM(B2:B9)</f>
-        <v>4281</v>
+        <v>4761</v>
       </c>
       <c r="C10">
         <f t="shared" ref="C10:F10" si="6">SUM(C2:C9)</f>
-        <v>756</v>
+        <v>799</v>
       </c>
       <c r="D10">
         <f t="shared" si="6"/>
-        <v>541882</v>
+        <v>669378</v>
       </c>
       <c r="E10">
         <f t="shared" si="6"/>
-        <v>3359775</v>
+        <v>4657695</v>
       </c>
       <c r="F10">
         <f t="shared" si="6"/>
-        <v>103556</v>
+        <v>115983</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="B12">
         <f>(8*D10-B10*C10)/SQRT((8*E10-B10^2)*(8*F10-C10^2))</f>
-        <v>0.74120916984356178</v>
+        <v>0.75460098090264371</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lets the MusicPlayer warm up
</commit_message>
<xml_diff>
--- a/HW4/Lines to Seconds stats.xlsx
+++ b/HW4/Lines to Seconds stats.xlsx
@@ -197,7 +197,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1592</c:v>
+                  <c:v>2535</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>897</c:v>
@@ -230,7 +230,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>166</c:v>
+                  <c:v>248</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>237</c:v>
@@ -296,7 +296,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1592</c:v>
+                  <c:v>2535</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>897</c:v>
@@ -329,28 +329,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>205.81522640233038</c:v>
+                  <c:v>275.00233775586145</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>131.95595884158342</c:v>
+                  <c:v>126.77562027830874</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71.274459881602851</c:v>
+                  <c:v>75.104401914644143</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42.580931476708358</c:v>
+                  <c:v>50.671426506256324</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>135.88803495632823</c:v>
+                  <c:v>130.12384283427298</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>69.255285660517686</c:v>
+                  <c:v>73.385044385905729</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57.671601971134351</c:v>
+                  <c:v>63.521361721038062</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>84.558500809794751</c:v>
+                  <c:v>86.415964603712567</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1394,7 +1394,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1415,34 +1415,34 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1592</v>
+        <v>2535</v>
       </c>
       <c r="C2">
-        <v>166</v>
+        <v>248</v>
       </c>
       <c r="D2">
         <f>B2*C2</f>
-        <v>264272</v>
+        <v>628680</v>
       </c>
       <c r="E2">
         <f>B2^2</f>
-        <v>2534464</v>
+        <v>6426225</v>
       </c>
       <c r="F2">
         <f>C2^2</f>
-        <v>27556</v>
+        <v>61504</v>
       </c>
       <c r="G2">
         <f t="shared" ref="G2:G7" si="0">G3</f>
-        <v>36.62968114087839</v>
+        <v>45.603846421553669</v>
       </c>
       <c r="H2">
         <f t="shared" ref="H2:H7" si="1">H3</f>
-        <v>0.10627232742553516</v>
+        <v>9.0492501512547452E-2</v>
       </c>
       <c r="I2">
         <f>G2+H2*B2</f>
-        <v>205.81522640233038</v>
+        <v>275.00233775586145</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1469,15 +1469,15 @@
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
-        <v>36.62968114087839</v>
+        <v>45.603846421553669</v>
       </c>
       <c r="H3">
         <f t="shared" si="1"/>
-        <v>0.10627232742553516</v>
+        <v>9.0492501512547452E-2</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I9" si="5">G3+H3*B3</f>
-        <v>131.95595884158342</v>
+        <v>126.77562027830874</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1504,15 +1504,15 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>36.62968114087839</v>
+        <v>45.603846421553669</v>
       </c>
       <c r="H4">
         <f t="shared" si="1"/>
-        <v>0.10627232742553516</v>
+        <v>9.0492501512547452E-2</v>
       </c>
       <c r="I4">
         <f t="shared" si="5"/>
-        <v>71.274459881602851</v>
+        <v>75.104401914644143</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1539,15 +1539,15 @@
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>36.62968114087839</v>
+        <v>45.603846421553669</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
-        <v>0.10627232742553516</v>
+        <v>9.0492501512547452E-2</v>
       </c>
       <c r="I5">
         <f t="shared" si="5"/>
-        <v>42.580931476708358</v>
+        <v>50.671426506256324</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1574,15 +1574,15 @@
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>36.62968114087839</v>
+        <v>45.603846421553669</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>0.10627232742553516</v>
+        <v>9.0492501512547452E-2</v>
       </c>
       <c r="I6">
         <f t="shared" si="5"/>
-        <v>135.88803495632823</v>
+        <v>130.12384283427298</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1609,15 +1609,15 @@
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>36.62968114087839</v>
+        <v>45.603846421553669</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>0.10627232742553516</v>
+        <v>9.0492501512547452E-2</v>
       </c>
       <c r="I7">
         <f t="shared" si="5"/>
-        <v>69.255285660517686</v>
+        <v>73.385044385905729</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1644,15 +1644,15 @@
       </c>
       <c r="G8">
         <f>G9</f>
-        <v>36.62968114087839</v>
+        <v>45.603846421553669</v>
       </c>
       <c r="H8">
         <f>H9</f>
-        <v>0.10627232742553516</v>
+        <v>9.0492501512547452E-2</v>
       </c>
       <c r="I8">
         <f t="shared" si="5"/>
-        <v>57.671601971134351</v>
+        <v>63.521361721038062</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1679,15 +1679,15 @@
       </c>
       <c r="G9">
         <f>C10/8-H9*B10/8</f>
-        <v>36.62968114087839</v>
+        <v>45.603846421553669</v>
       </c>
       <c r="H9">
         <f>(8*D10-B10*C10)/(8*E10-B10^2)</f>
-        <v>0.10627232742553516</v>
+        <v>9.0492501512547452E-2</v>
       </c>
       <c r="I9">
         <f t="shared" si="5"/>
-        <v>84.558500809794751</v>
+        <v>86.415964603712567</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1696,23 +1696,23 @@
       </c>
       <c r="B10">
         <f>SUM(B2:B9)</f>
-        <v>4761</v>
+        <v>5704</v>
       </c>
       <c r="C10">
         <f t="shared" ref="C10:F10" si="6">SUM(C2:C9)</f>
-        <v>799</v>
+        <v>881</v>
       </c>
       <c r="D10">
         <f t="shared" si="6"/>
-        <v>669378</v>
+        <v>1033786</v>
       </c>
       <c r="E10">
         <f t="shared" si="6"/>
-        <v>4657695</v>
+        <v>8549456</v>
       </c>
       <c r="F10">
         <f t="shared" si="6"/>
-        <v>115983</v>
+        <v>149931</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="B12">
         <f>(8*D10-B10*C10)/SQRT((8*E10-B10^2)*(8*F10-C10^2))</f>
-        <v>0.75460098090264371</v>
+        <v>0.83291458078173075</v>
       </c>
     </row>
   </sheetData>

</xml_diff>